<commit_message>
tariff model added with db_util
</commit_message>
<xml_diff>
--- a/data/raw/sample_bill.xlsx
+++ b/data/raw/sample_bill.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubuffalo-my.sharepoint.com/personal/hpatil2_buffalo_edu/Documents/Desktop/MS/2.Course/4.Third_Fourth Semester/CDA 500/Troy &amp; Banks/Code_Base/utility-billing-ai/data/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_FFC65FC04D812F52C74DB7B6A2B5BA7543FE3061" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E6957A2-F8CB-FD44-976F-A3C2A36312B1}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="32460" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -553,8 +559,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,13 +606,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -644,7 +658,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -678,6 +692,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -712,9 +727,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -887,14 +903,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>99</v>
       </c>
@@ -991,7 +1026,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>100</v>
       </c>
@@ -1038,7 +1073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>101</v>
       </c>
@@ -1085,7 +1120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>102</v>
       </c>
@@ -1132,7 +1167,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>103</v>
       </c>
@@ -1179,7 +1214,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>104</v>
       </c>
@@ -1226,7 +1261,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>105</v>
       </c>
@@ -1273,7 +1308,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>106</v>
       </c>
@@ -1320,7 +1355,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>107</v>
       </c>
@@ -1367,7 +1402,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>108</v>
       </c>
@@ -1414,7 +1449,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>109</v>
       </c>
@@ -1461,7 +1496,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>110</v>
       </c>
@@ -1508,7 +1543,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>111</v>
       </c>
@@ -1555,7 +1590,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>112</v>
       </c>
@@ -1602,7 +1637,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>113</v>
       </c>
@@ -1649,7 +1684,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>114</v>
       </c>
@@ -1696,7 +1731,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>115</v>
       </c>
@@ -1743,7 +1778,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>116</v>
       </c>
@@ -1790,7 +1825,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>117</v>
       </c>
@@ -1837,7 +1872,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>118</v>
       </c>
@@ -1884,7 +1919,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>119</v>
       </c>
@@ -1931,7 +1966,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>120</v>
       </c>
@@ -1978,7 +2013,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>121</v>
       </c>
@@ -2025,7 +2060,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>122</v>
       </c>
@@ -2072,7 +2107,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>123</v>
       </c>
@@ -2119,7 +2154,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>124</v>
       </c>
@@ -2166,7 +2201,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>125</v>
       </c>
@@ -2213,7 +2248,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>126</v>
       </c>
@@ -2260,7 +2295,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>127</v>
       </c>
@@ -2307,7 +2342,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>128</v>
       </c>
@@ -2354,7 +2389,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>129</v>
       </c>
@@ -2401,7 +2436,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>130</v>
       </c>
@@ -2448,7 +2483,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>131</v>
       </c>
@@ -2495,7 +2530,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>132</v>
       </c>
@@ -2542,7 +2577,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>133</v>
       </c>
@@ -2589,7 +2624,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>134</v>
       </c>
@@ -2636,7 +2671,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>135</v>
       </c>
@@ -2683,7 +2718,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>136</v>
       </c>
@@ -2730,7 +2765,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>137</v>
       </c>

</xml_diff>